<commit_message>
adding div class to excel
</commit_message>
<xml_diff>
--- a/welcome-page-icons.xlsx
+++ b/welcome-page-icons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Rony\web0\GP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F057312E-1E5A-446C-A402-FEA9104C1DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CAFC88-F0C6-4FB3-8C53-2882507CA76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>1</t>
   </si>
@@ -50,6 +50,21 @@
   </si>
   <si>
     <t>Elevate</t>
+  </si>
+  <si>
+    <t>ri-store-line</t>
+  </si>
+  <si>
+    <t>ri-bar-chart-box-line</t>
+  </si>
+  <si>
+    <t>ri-calendar-todo-line</t>
+  </si>
+  <si>
+    <t>ri-paint-brush-line</t>
+  </si>
+  <si>
+    <t>ri-database-2-line</t>
   </si>
 </sst>
 </file>
@@ -388,56 +403,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>